<commit_message>
Implemented READ / WRITE XLS
</commit_message>
<xml_diff>
--- a/dbpa/src/test/resources/data/problem.xlsx
+++ b/dbpa/src/test/resources/data/problem.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFBB60D-6309-4715-B9F9-A5E355733930}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B788DCF-1329-4E0C-A690-685595D39553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6570" yWindow="705" windowWidth="20865" windowHeight="13845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,64 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
-  <si>
-    <r>
-      <t xml:space="preserve">Corporate Transportation Group
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">335 Bond St.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Brooklyn, NY 11231
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Tel. (718) 643-3900</t>
-    </r>
-  </si>
-  <si>
-    <t>Check No: 2276922</t>
-  </si>
-  <si>
-    <t>CREATIVE MOBILE TECHNOLOGIES, LLC</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>Check Date: 06/29/2019</t>
   </si>
   <si>
-    <t>4232 21ST STREET</t>
-  </si>
-  <si>
-    <t>Check Amt: $102,876.34</t>
-  </si>
-  <si>
-    <t>LIC, NY 11101</t>
-  </si>
-  <si>
     <t>Dr.Id: 2510   Car#: 2510</t>
   </si>
   <si>
@@ -140,63 +87,24 @@
     <t>2019-06-26 00:14:00</t>
   </si>
   <si>
-    <t>THOMPSON,KENNY</t>
-  </si>
-  <si>
-    <t>342 THROOP AVE, BROOKLYN, NY 11206</t>
-  </si>
-  <si>
-    <t>18 E 53 ST, BROOKLYN, NY 11203</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MTA       </t>
-  </si>
-  <si>
     <t>27694425</t>
   </si>
   <si>
     <t>2019-06-26 01:00:00</t>
   </si>
   <si>
-    <t>ROWLAND,TRACY</t>
-  </si>
-  <si>
-    <t>490 PACIFIC ST, BROOKLYN, NY 11217</t>
-  </si>
-  <si>
-    <t>1009 E 37 ST, BROOKLYN, NY 11210</t>
-  </si>
-  <si>
-    <t>INDERJEET,TEJRANI</t>
-  </si>
-  <si>
     <t>27721981</t>
   </si>
   <si>
     <t>2019-06-27 20:40:00</t>
   </si>
   <si>
-    <t>SARPONG,REGINA</t>
-  </si>
-  <si>
-    <t>1579 METROPOLITAN AVE, , NY 10462</t>
-  </si>
-  <si>
-    <t>54 FEATHERBED LA, , NY 10453</t>
-  </si>
-  <si>
     <t>27727897</t>
   </si>
   <si>
     <t>2019-06-27 22:25:00</t>
   </si>
   <si>
-    <t>83 RIVINGTON ST, , NY 10002</t>
-  </si>
-  <si>
-    <t>30 3 AVE, , NY 11217</t>
-  </si>
-  <si>
     <t>YTD Tolls</t>
   </si>
   <si>
@@ -210,6 +118,51 @@
   </si>
   <si>
     <t>YTD Net</t>
+  </si>
+  <si>
+    <t>Nonsense Technology Company
+123 Smurf St.
+Wazoo, XY 12345
+Tel. (555) 555-1212</t>
+  </si>
+  <si>
+    <t>Check No: K9112233</t>
+  </si>
+  <si>
+    <t>Check Amt: $0.34</t>
+  </si>
+  <si>
+    <t>YET ANOTHER TECH COMANY, LLC</t>
+  </si>
+  <si>
+    <t>1234 56ST STREET</t>
+  </si>
+  <si>
+    <t>Asphalt, BC 98765</t>
+  </si>
+  <si>
+    <t>CARTMAN, ERIC</t>
+  </si>
+  <si>
+    <t>MORGAN,TRACY</t>
+  </si>
+  <si>
+    <t>SPAGHETTI,REGINA</t>
+  </si>
+  <si>
+    <t>JUMANJI,TEJRANI</t>
+  </si>
+  <si>
+    <t>123 DIRT AVE, BROOKLYN, NY 11206</t>
+  </si>
+  <si>
+    <t>456 HELL ST, BROOKLYN, NY 11217</t>
+  </si>
+  <si>
+    <t>7890 INFERNO AVE, , NY 10462</t>
+  </si>
+  <si>
+    <t>99 NINETYNINE ST, , NY 10002</t>
   </si>
 </sst>
 </file>
@@ -438,6 +391,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
@@ -450,25 +408,20 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -965,7 +918,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AG40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1007,37 +962,37 @@
   <sheetData>
     <row r="1" spans="2:24" ht="6.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:24" ht="1.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
     </row>
     <row r="3" spans="2:24" ht="0.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
       <c r="F3" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
+        <v>34</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
       <c r="U3" s="1"/>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
       <c r="X3" s="3"/>
     </row>
     <row r="4" spans="2:24" ht="2.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
       <c r="M4" s="30" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="N4" s="31"/>
       <c r="O4" s="31"/>
@@ -1048,123 +1003,123 @@
       <c r="X4" s="5"/>
     </row>
     <row r="5" spans="2:24" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
       <c r="M5" s="33"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
       <c r="R5" s="24"/>
       <c r="U5" s="4"/>
       <c r="V5" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="W5" s="21"/>
+        <v>37</v>
+      </c>
+      <c r="W5" s="15"/>
       <c r="X5" s="24"/>
     </row>
     <row r="6" spans="2:24" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
       <c r="M6" s="4"/>
       <c r="R6" s="5"/>
       <c r="U6" s="4"/>
       <c r="V6" s="28"/>
-      <c r="W6" s="21"/>
+      <c r="W6" s="15"/>
       <c r="X6" s="24"/>
     </row>
     <row r="7" spans="2:24" ht="0.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
       <c r="M7" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
       <c r="R7" s="24"/>
       <c r="U7" s="4"/>
       <c r="V7" s="28"/>
-      <c r="W7" s="21"/>
+      <c r="W7" s="15"/>
       <c r="X7" s="24"/>
     </row>
     <row r="8" spans="2:24" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
       <c r="M8" s="25"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
       <c r="R8" s="24"/>
       <c r="U8" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="V8" s="21"/>
-      <c r="W8" s="21"/>
+        <v>38</v>
+      </c>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
       <c r="X8" s="24"/>
     </row>
     <row r="9" spans="2:24" ht="0.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
       <c r="M9" s="4"/>
       <c r="R9" s="5"/>
       <c r="U9" s="25"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="21"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
       <c r="X9" s="24"/>
     </row>
     <row r="10" spans="2:24" ht="0.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
       <c r="M10" s="4"/>
       <c r="R10" s="5"/>
       <c r="U10" s="4"/>
       <c r="X10" s="5"/>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
       <c r="M11" s="4"/>
       <c r="R11" s="5"/>
       <c r="U11" s="4"/>
@@ -1178,26 +1133,26 @@
     </row>
     <row r="13" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M13" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="21"/>
+        <v>36</v>
+      </c>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
       <c r="R13" s="24"/>
       <c r="U13" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="V13" s="21"/>
-      <c r="W13" s="21"/>
+        <v>39</v>
+      </c>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
       <c r="X13" s="24"/>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.2">
       <c r="M14" s="25"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="21"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
       <c r="R14" s="24"/>
       <c r="U14" s="4"/>
       <c r="X14" s="5"/>
@@ -1216,33 +1171,33 @@
       <c r="Q16" s="7"/>
       <c r="R16" s="8"/>
       <c r="U16" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="V16" s="21"/>
-      <c r="W16" s="21"/>
+        <v>1</v>
+      </c>
+      <c r="V16" s="15"/>
+      <c r="W16" s="15"/>
       <c r="X16" s="24"/>
     </row>
     <row r="17" spans="4:33" x14ac:dyDescent="0.2">
       <c r="U17" s="25"/>
-      <c r="V17" s="21"/>
-      <c r="W17" s="21"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="15"/>
       <c r="X17" s="24"/>
     </row>
     <row r="18" spans="4:33" x14ac:dyDescent="0.2">
       <c r="D18" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
+        <v>2</v>
+      </c>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
       <c r="U18" s="25"/>
-      <c r="V18" s="21"/>
-      <c r="W18" s="21"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="15"/>
       <c r="X18" s="24"/>
     </row>
     <row r="19" spans="4:33" x14ac:dyDescent="0.2">
       <c r="D19" s="28"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
       <c r="U19" s="6"/>
       <c r="V19" s="7"/>
       <c r="W19" s="7"/>
@@ -1251,187 +1206,177 @@
     <row r="20" spans="4:33" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="4:33" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="4:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D22" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="P22" s="16"/>
+      <c r="D22" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="P22" s="18"/>
     </row>
     <row r="23" spans="4:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D23" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="17">
+      <c r="D23" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="22">
         <v>1.3</v>
       </c>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="17">
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="22">
         <v>16.899999999999999</v>
       </c>
-      <c r="P23" s="16"/>
+      <c r="P23" s="18"/>
     </row>
     <row r="24" spans="4:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D24" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="17">
+      <c r="D24" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="22">
         <v>1.3</v>
       </c>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="16"/>
-      <c r="O24" s="17">
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="22">
         <v>16.899999999999999</v>
       </c>
-      <c r="P24" s="16"/>
+      <c r="P24" s="18"/>
     </row>
     <row r="25" spans="4:33" ht="12.2" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="4:33" ht="0.6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="4:33" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D27" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
+      <c r="D27" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
     </row>
     <row r="28" spans="4:33" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="4:33" ht="3.95" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="4:33" x14ac:dyDescent="0.2">
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="O30" s="17"/>
+      <c r="P30" s="17"/>
+      <c r="Q30" s="17"/>
+      <c r="R30" s="17"/>
+      <c r="S30" s="18"/>
+      <c r="T30" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="U30" s="17"/>
+      <c r="V30" s="17"/>
+      <c r="W30" s="17"/>
+      <c r="X30" s="17"/>
+      <c r="Y30" s="18"/>
+      <c r="Z30" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA30" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB30" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="22" t="s">
+      <c r="AC30" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="22" t="s">
+      <c r="AD30" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="15"/>
-      <c r="S30" s="16"/>
-      <c r="T30" s="22" t="s">
+      <c r="AE30" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="U30" s="15"/>
-      <c r="V30" s="15"/>
-      <c r="W30" s="15"/>
-      <c r="X30" s="15"/>
-      <c r="Y30" s="16"/>
-      <c r="Z30" s="12" t="s">
+      <c r="AF30" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="AA30" s="9" t="s">
+      <c r="AG30" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="AB30" s="9" t="s">
+    </row>
+    <row r="31" spans="4:33" x14ac:dyDescent="0.2">
+      <c r="D31" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="AC30" s="9" t="s">
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="AD30" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE30" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AF30" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="AG30" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="4:33" x14ac:dyDescent="0.2">
-      <c r="D31" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="16"/>
-      <c r="N31" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="15"/>
-      <c r="R31" s="15"/>
-      <c r="S31" s="16"/>
-      <c r="T31" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="U31" s="15"/>
-      <c r="V31" s="15"/>
-      <c r="W31" s="15"/>
-      <c r="X31" s="15"/>
-      <c r="Y31" s="16"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="O31" s="17"/>
+      <c r="P31" s="17"/>
+      <c r="Q31" s="17"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="18"/>
+      <c r="T31" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="U31" s="17"/>
+      <c r="V31" s="17"/>
+      <c r="W31" s="17"/>
+      <c r="X31" s="17"/>
+      <c r="Y31" s="18"/>
       <c r="Z31" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA31" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB31" s="11">
-        <v>28.22</v>
-      </c>
-      <c r="AC31" s="11">
-        <v>0</v>
-      </c>
-      <c r="AD31" s="11">
-        <v>1</v>
-      </c>
-      <c r="AE31" s="11">
-        <v>0</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="AA31" s="13"/>
+      <c r="AB31" s="11"/>
+      <c r="AC31" s="11"/>
+      <c r="AD31" s="11"/>
+      <c r="AE31" s="11"/>
       <c r="AF31" s="11">
         <v>1.41</v>
       </c>
@@ -1440,54 +1385,44 @@
       </c>
     </row>
     <row r="32" spans="4:33" x14ac:dyDescent="0.2">
-      <c r="D32" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="O32" s="15"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="15"/>
-      <c r="S32" s="16"/>
-      <c r="T32" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="U32" s="15"/>
-      <c r="V32" s="15"/>
-      <c r="W32" s="15"/>
-      <c r="X32" s="15"/>
-      <c r="Y32" s="16"/>
+      <c r="D32" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="18"/>
+      <c r="T32" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="U32" s="17"/>
+      <c r="V32" s="17"/>
+      <c r="W32" s="17"/>
+      <c r="X32" s="17"/>
+      <c r="Y32" s="18"/>
       <c r="Z32" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA32" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB32" s="11">
-        <v>35.340000000000003</v>
-      </c>
-      <c r="AC32" s="11">
-        <v>0</v>
-      </c>
-      <c r="AD32" s="11">
-        <v>1</v>
-      </c>
-      <c r="AE32" s="11">
-        <v>0</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="AA32" s="13"/>
+      <c r="AB32" s="11"/>
+      <c r="AC32" s="11"/>
+      <c r="AD32" s="11"/>
+      <c r="AE32" s="11"/>
       <c r="AF32" s="11">
         <v>1.77</v>
       </c>
@@ -1496,54 +1431,44 @@
       </c>
     </row>
     <row r="33" spans="3:33" x14ac:dyDescent="0.2">
-      <c r="D33" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="16"/>
-      <c r="N33" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="15"/>
-      <c r="R33" s="15"/>
-      <c r="S33" s="16"/>
-      <c r="T33" s="19" t="s">
+      <c r="D33" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="U33" s="15"/>
-      <c r="V33" s="15"/>
-      <c r="W33" s="15"/>
-      <c r="X33" s="15"/>
-      <c r="Y33" s="16"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="17"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="18"/>
+      <c r="T33" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="U33" s="17"/>
+      <c r="V33" s="17"/>
+      <c r="W33" s="17"/>
+      <c r="X33" s="17"/>
+      <c r="Y33" s="18"/>
       <c r="Z33" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA33" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB33" s="11">
-        <v>18.86</v>
-      </c>
-      <c r="AC33" s="11">
-        <v>0</v>
-      </c>
-      <c r="AD33" s="11">
-        <v>1</v>
-      </c>
-      <c r="AE33" s="11">
-        <v>0</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="AA33" s="13"/>
+      <c r="AB33" s="11"/>
+      <c r="AC33" s="11"/>
+      <c r="AD33" s="11"/>
+      <c r="AE33" s="11"/>
       <c r="AF33" s="11">
         <v>0.94</v>
       </c>
@@ -1552,54 +1477,44 @@
       </c>
     </row>
     <row r="34" spans="3:33" x14ac:dyDescent="0.2">
-      <c r="D34" s="18" t="s">
+      <c r="D34" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="O34" s="17"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="17"/>
+      <c r="R34" s="17"/>
+      <c r="S34" s="18"/>
+      <c r="T34" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="U34" s="17"/>
+      <c r="V34" s="17"/>
+      <c r="W34" s="17"/>
+      <c r="X34" s="17"/>
+      <c r="Y34" s="18"/>
+      <c r="Z34" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="16"/>
-      <c r="N34" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="O34" s="15"/>
-      <c r="P34" s="15"/>
-      <c r="Q34" s="15"/>
-      <c r="R34" s="15"/>
-      <c r="S34" s="16"/>
-      <c r="T34" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="U34" s="15"/>
-      <c r="V34" s="15"/>
-      <c r="W34" s="15"/>
-      <c r="X34" s="15"/>
-      <c r="Y34" s="16"/>
-      <c r="Z34" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA34" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB34" s="11">
-        <v>25.52</v>
-      </c>
-      <c r="AC34" s="11">
-        <v>0</v>
-      </c>
-      <c r="AD34" s="11">
-        <v>1</v>
-      </c>
-      <c r="AE34" s="11">
-        <v>0</v>
-      </c>
+      <c r="AA34" s="13"/>
+      <c r="AB34" s="11"/>
+      <c r="AC34" s="11"/>
+      <c r="AD34" s="11"/>
+      <c r="AE34" s="11"/>
       <c r="AF34" s="11">
         <v>1.28</v>
       </c>
@@ -1608,30 +1523,30 @@
       </c>
     </row>
     <row r="35" spans="3:33" x14ac:dyDescent="0.2">
-      <c r="D35" s="18"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="16"/>
-      <c r="N35" s="19"/>
-      <c r="O35" s="15"/>
-      <c r="P35" s="15"/>
-      <c r="Q35" s="15"/>
-      <c r="R35" s="15"/>
-      <c r="S35" s="16"/>
-      <c r="T35" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="U35" s="15"/>
-      <c r="V35" s="15"/>
-      <c r="W35" s="15"/>
-      <c r="X35" s="15"/>
-      <c r="Y35" s="16"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="21"/>
+      <c r="O35" s="17"/>
+      <c r="P35" s="17"/>
+      <c r="Q35" s="17"/>
+      <c r="R35" s="17"/>
+      <c r="S35" s="18"/>
+      <c r="T35" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="U35" s="17"/>
+      <c r="V35" s="17"/>
+      <c r="W35" s="17"/>
+      <c r="X35" s="17"/>
+      <c r="Y35" s="18"/>
       <c r="Z35" s="10"/>
       <c r="AA35" s="13"/>
       <c r="AB35" s="11">
@@ -1656,104 +1571,68 @@
     <row r="36" spans="3:33" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="37" spans="3:33" ht="30.95" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="3:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C38" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="J38" s="16"/>
-      <c r="L38" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="16"/>
+      <c r="C38" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J38" s="18"/>
+      <c r="L38" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="M38" s="17"/>
+      <c r="N38" s="17"/>
+      <c r="O38" s="18"/>
       <c r="P38" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="R38" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="S38" s="15"/>
-      <c r="T38" s="15"/>
-      <c r="U38" s="15"/>
-      <c r="V38" s="16"/>
+        <v>32</v>
+      </c>
+      <c r="R38" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="S38" s="17"/>
+      <c r="T38" s="17"/>
+      <c r="U38" s="17"/>
+      <c r="V38" s="18"/>
     </row>
     <row r="39" spans="3:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C39" s="17">
+      <c r="C39" s="22">
         <v>0</v>
       </c>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="17">
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="22">
         <v>0</v>
       </c>
-      <c r="J39" s="16"/>
-      <c r="L39" s="17">
+      <c r="J39" s="18"/>
+      <c r="L39" s="22">
         <v>2754646.94</v>
       </c>
-      <c r="M39" s="15"/>
-      <c r="N39" s="15"/>
-      <c r="O39" s="16"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="18"/>
       <c r="P39" s="11">
         <v>137732.35</v>
       </c>
-      <c r="R39" s="17">
+      <c r="R39" s="22">
         <v>2523496.15</v>
       </c>
-      <c r="S39" s="15"/>
-      <c r="T39" s="15"/>
-      <c r="U39" s="15"/>
-      <c r="V39" s="16"/>
+      <c r="S39" s="17"/>
+      <c r="T39" s="17"/>
+      <c r="U39" s="17"/>
+      <c r="V39" s="18"/>
     </row>
     <row r="40" spans="3:33" ht="53.45" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="D27:I27"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="N30:S30"/>
-    <mergeCell ref="T30:Y30"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="N31:S31"/>
-    <mergeCell ref="T31:Y31"/>
-    <mergeCell ref="D23:I23"/>
-    <mergeCell ref="J23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="D24:I24"/>
-    <mergeCell ref="J24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="M13:R14"/>
-    <mergeCell ref="U13:X13"/>
-    <mergeCell ref="U16:X18"/>
-    <mergeCell ref="D18:F19"/>
-    <mergeCell ref="D22:I22"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="B2:D10"/>
-    <mergeCell ref="F3:J11"/>
-    <mergeCell ref="M4:R5"/>
-    <mergeCell ref="V5:X7"/>
-    <mergeCell ref="M7:R8"/>
-    <mergeCell ref="U8:X9"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="H32:M32"/>
-    <mergeCell ref="N32:S32"/>
-    <mergeCell ref="T32:Y32"/>
-    <mergeCell ref="C38:H38"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="L38:O38"/>
-    <mergeCell ref="R38:V38"/>
     <mergeCell ref="C39:H39"/>
     <mergeCell ref="I39:J39"/>
     <mergeCell ref="L39:O39"/>
@@ -1766,10 +1645,46 @@
     <mergeCell ref="H35:M35"/>
     <mergeCell ref="N35:S35"/>
     <mergeCell ref="T35:Y35"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="N32:S32"/>
+    <mergeCell ref="T32:Y32"/>
+    <mergeCell ref="C38:H38"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="L38:O38"/>
+    <mergeCell ref="R38:V38"/>
     <mergeCell ref="D33:G33"/>
     <mergeCell ref="H33:M33"/>
     <mergeCell ref="N33:S33"/>
     <mergeCell ref="T33:Y33"/>
+    <mergeCell ref="B2:D10"/>
+    <mergeCell ref="F3:J11"/>
+    <mergeCell ref="M4:R5"/>
+    <mergeCell ref="V5:X7"/>
+    <mergeCell ref="M7:R8"/>
+    <mergeCell ref="U8:X9"/>
+    <mergeCell ref="M13:R14"/>
+    <mergeCell ref="U13:X13"/>
+    <mergeCell ref="U16:X18"/>
+    <mergeCell ref="D18:F19"/>
+    <mergeCell ref="D22:I22"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="N31:S31"/>
+    <mergeCell ref="T31:Y31"/>
+    <mergeCell ref="D23:I23"/>
+    <mergeCell ref="J23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="D24:I24"/>
+    <mergeCell ref="J24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="D27:I27"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="N30:S30"/>
+    <mergeCell ref="T30:Y30"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.1" right="0.1" top="0.15000000000000002" bottom="0.55625000000000002" header="0.15000000000000002" footer="0.15000000000000002"/>

</xml_diff>